<commit_message>
update migration for capaian
</commit_message>
<xml_diff>
--- a/database/Database Library SO KPI SI versi 3.0.xlsx
+++ b/database/Database Library SO KPI SI versi 3.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dicha\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B5F63A-B0C6-49C7-B317-0AFE7141BC10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C32C72-7B63-423D-B214-B15B8F9B70AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{12A28D7E-AFF8-4833-A78C-08CB9826905C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="181">
   <si>
     <t>Business Categories</t>
   </si>
@@ -553,12 +553,6 @@
   </si>
   <si>
     <t>Pelanggan</t>
-  </si>
-  <si>
-    <t>Rupiah</t>
-  </si>
-  <si>
-    <t>Nominal</t>
   </si>
   <si>
     <t>Bisnis</t>
@@ -1040,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A759BA-9F1D-47A0-BED0-E899B8478BC5}">
   <dimension ref="B2:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1067,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>160</v>
@@ -1082,7 +1076,7 @@
         <v>161</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>9</v>
@@ -1111,7 +1105,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>171</v>
@@ -1126,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>6</v>
@@ -1342,10 +1336,10 @@
         <v>46</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>177</v>
+        <v>12</v>
       </c>
       <c r="L9" s="8" t="s">
         <v>14</v>
@@ -1370,10 +1364,10 @@
         <v>47</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L10" s="8" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Revisi add KPI edit KPI pasca penambahan periode_th
</commit_message>
<xml_diff>
--- a/database/Database Library SO KPI SI versi 3.0.xlsx
+++ b/database/Database Library SO KPI SI versi 3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C32C72-7B63-423D-B214-B15B8F9B70AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EA4D17-F99A-458A-BAC6-89EFBE900E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{12A28D7E-AFF8-4833-A78C-08CB9826905C}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="9072" xr2:uid="{12A28D7E-AFF8-4833-A78C-08CB9826905C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A759BA-9F1D-47A0-BED0-E899B8478BC5}">
   <dimension ref="B2:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
update Aspect and Bisnis filter pada form add SO
</commit_message>
<xml_diff>
--- a/database/Database Library SO KPI SI versi 3.0.xlsx
+++ b/database/Database Library SO KPI SI versi 3.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EA4D17-F99A-458A-BAC6-89EFBE900E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0760D3-A134-4ADA-A16B-434128823199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="9072" xr2:uid="{12A28D7E-AFF8-4833-A78C-08CB9826905C}"/>
+    <workbookView xWindow="1776" yWindow="1776" windowWidth="17280" windowHeight="9072" xr2:uid="{12A28D7E-AFF8-4833-A78C-08CB9826905C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="186">
   <si>
     <t>Business Categories</t>
   </si>
@@ -561,13 +561,28 @@
     <t>Jenis Pilihan KPI</t>
   </si>
   <si>
-    <t>Apakah Transportasi/gudang/Warehouses</t>
-  </si>
-  <si>
-    <t>Produktivitas/Waktu/Time dll</t>
-  </si>
-  <si>
     <t>Aspect</t>
+  </si>
+  <si>
+    <t>Distribusi</t>
+  </si>
+  <si>
+    <t>Pergudangan</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Transportasi</t>
+  </si>
+  <si>
+    <t>Produktifitas</t>
+  </si>
+  <si>
+    <t>Kualitas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keuangan/Produktivitas </t>
   </si>
 </sst>
 </file>
@@ -1034,8 +1049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A759BA-9F1D-47A0-BED0-E899B8478BC5}">
   <dimension ref="B2:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1079,7 @@
         <v>176</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>160</v>
@@ -1100,12 +1115,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>171</v>
@@ -1120,7 +1135,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>6</v>
@@ -1144,7 +1159,9 @@
     </row>
     <row r="4" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B4" s="6"/>
-      <c r="C4" s="17"/>
+      <c r="C4" s="17" t="s">
+        <v>180</v>
+      </c>
       <c r="D4" s="16" t="s">
         <v>171</v>
       </c>
@@ -1157,7 +1174,9 @@
       <c r="G4" s="13">
         <v>2</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1180,7 +1199,9 @@
     </row>
     <row r="5" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
-      <c r="C5" s="17"/>
+      <c r="C5" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D5" s="16" t="s">
         <v>172</v>
       </c>
@@ -1193,7 +1214,9 @@
       <c r="G5" s="13">
         <v>3</v>
       </c>
-      <c r="H5" s="13"/>
+      <c r="H5" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I5" s="8" t="s">
         <v>8</v>
       </c>
@@ -1216,7 +1239,9 @@
     </row>
     <row r="6" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B6" s="6"/>
-      <c r="C6" s="17"/>
+      <c r="C6" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="D6" s="16" t="s">
         <v>171</v>
       </c>
@@ -1229,7 +1254,9 @@
       <c r="G6" s="13">
         <v>4</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I6" s="8" t="s">
         <v>43</v>
       </c>
@@ -1250,7 +1277,9 @@
     </row>
     <row r="7" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6"/>
-      <c r="C7" s="17"/>
+      <c r="C7" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="D7" s="16" t="s">
         <v>171</v>
       </c>
@@ -1263,7 +1292,9 @@
       <c r="G7" s="13">
         <v>5</v>
       </c>
-      <c r="H7" s="13"/>
+      <c r="H7" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I7" s="7" t="s">
         <v>44</v>
       </c>
@@ -1284,7 +1315,9 @@
     </row>
     <row r="8" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="6"/>
-      <c r="C8" s="17"/>
+      <c r="C8" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="D8" s="16" t="s">
         <v>171</v>
       </c>
@@ -1297,7 +1330,9 @@
       <c r="G8" s="13">
         <v>6</v>
       </c>
-      <c r="H8" s="13"/>
+      <c r="H8" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I8" s="7" t="s">
         <v>45</v>
       </c>
@@ -1318,7 +1353,9 @@
     </row>
     <row r="9" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="6"/>
-      <c r="C9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D9" s="16" t="s">
         <v>173</v>
       </c>
@@ -1331,7 +1368,9 @@
       <c r="G9" s="13">
         <v>7</v>
       </c>
-      <c r="H9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I9" s="7" t="s">
         <v>46</v>
       </c>
@@ -1359,7 +1398,9 @@
       <c r="G10" s="13">
         <v>8</v>
       </c>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I10" s="7" t="s">
         <v>47</v>
       </c>
@@ -1380,7 +1421,9 @@
     </row>
     <row r="11" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="6"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="D11" s="16" t="s">
         <v>171</v>
       </c>
@@ -1393,7 +1436,9 @@
       <c r="G11" s="13">
         <v>9</v>
       </c>
-      <c r="H11" s="13"/>
+      <c r="H11" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I11" s="7" t="s">
         <v>48</v>
       </c>
@@ -1414,9 +1459,11 @@
       </c>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="6"/>
-      <c r="C12" s="17"/>
+      <c r="C12" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D12" s="16" t="s">
         <v>174</v>
       </c>
@@ -1429,7 +1476,9 @@
       <c r="G12" s="13">
         <v>10</v>
       </c>
-      <c r="H12" s="13"/>
+      <c r="H12" s="13" t="s">
+        <v>185</v>
+      </c>
       <c r="I12" s="7" t="s">
         <v>49</v>
       </c>
@@ -1450,7 +1499,9 @@
     </row>
     <row r="13" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="6"/>
-      <c r="C13" s="17"/>
+      <c r="C13" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="D13" s="16" t="s">
         <v>175</v>
       </c>
@@ -1463,7 +1514,9 @@
       <c r="G13" s="13">
         <v>11</v>
       </c>
-      <c r="H13" s="13"/>
+      <c r="H13" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I13" s="7" t="s">
         <v>50</v>
       </c>
@@ -1484,7 +1537,9 @@
     </row>
     <row r="14" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="6"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="D14" s="16" t="s">
         <v>171</v>
       </c>
@@ -1497,7 +1552,9 @@
       <c r="G14" s="13">
         <v>12</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I14" s="7" t="s">
         <v>51</v>
       </c>
@@ -1518,7 +1575,9 @@
     </row>
     <row r="15" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15" s="6"/>
-      <c r="C15" s="17"/>
+      <c r="C15" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="D15" s="16" t="s">
         <v>171</v>
       </c>
@@ -1531,7 +1590,9 @@
       <c r="G15" s="13">
         <v>13</v>
       </c>
-      <c r="H15" s="13"/>
+      <c r="H15" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I15" s="7" t="s">
         <v>52</v>
       </c>
@@ -1556,7 +1617,9 @@
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="6"/>
-      <c r="C16" s="17"/>
+      <c r="C16" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D16" s="16"/>
       <c r="E16" s="14">
         <v>13</v>
@@ -1567,7 +1630,9 @@
       <c r="G16" s="13">
         <v>14</v>
       </c>
-      <c r="H16" s="13"/>
+      <c r="H16" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I16" s="7" t="s">
         <v>53</v>
       </c>
@@ -1590,7 +1655,9 @@
     </row>
     <row r="17" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B17" s="6"/>
-      <c r="C17" s="17"/>
+      <c r="C17" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D17" s="16" t="s">
         <v>175</v>
       </c>
@@ -1603,7 +1670,9 @@
       <c r="G17" s="13">
         <v>15</v>
       </c>
-      <c r="H17" s="13"/>
+      <c r="H17" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I17" s="7" t="s">
         <v>54</v>
       </c>
@@ -1622,7 +1691,9 @@
     </row>
     <row r="18" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B18" s="6"/>
-      <c r="C18" s="17"/>
+      <c r="C18" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D18" s="16" t="s">
         <v>173</v>
       </c>
@@ -1635,7 +1706,9 @@
       <c r="G18" s="13">
         <v>16</v>
       </c>
-      <c r="H18" s="13"/>
+      <c r="H18" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I18" s="7" t="s">
         <v>55</v>
       </c>
@@ -1656,7 +1729,9 @@
     </row>
     <row r="19" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
-      <c r="C19" s="17"/>
+      <c r="C19" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D19" s="16" t="s">
         <v>171</v>
       </c>
@@ -1669,7 +1744,9 @@
       <c r="G19" s="13">
         <v>17</v>
       </c>
-      <c r="H19" s="13"/>
+      <c r="H19" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I19" s="7" t="s">
         <v>56</v>
       </c>
@@ -1690,14 +1767,18 @@
     </row>
     <row r="20" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="6"/>
-      <c r="C20" s="17"/>
+      <c r="C20" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="D20" s="16"/>
       <c r="E20" s="14"/>
       <c r="F20" s="11"/>
       <c r="G20" s="13">
         <v>18</v>
       </c>
-      <c r="H20" s="13"/>
+      <c r="H20" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I20" s="7" t="s">
         <v>57</v>
       </c>
@@ -1718,7 +1799,9 @@
     </row>
     <row r="21" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-      <c r="C21" s="18"/>
+      <c r="C21" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D21" s="16" t="s">
         <v>174</v>
       </c>
@@ -1731,7 +1814,9 @@
       <c r="G21" s="13">
         <v>19</v>
       </c>
-      <c r="H21" s="13"/>
+      <c r="H21" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I21" s="7" t="s">
         <v>58</v>
       </c>
@@ -1756,7 +1841,9 @@
     </row>
     <row r="22" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-      <c r="C22" s="18"/>
+      <c r="C22" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D22" s="16" t="s">
         <v>172</v>
       </c>
@@ -1769,7 +1856,9 @@
       <c r="G22" s="13">
         <v>20</v>
       </c>
-      <c r="H22" s="13"/>
+      <c r="H22" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I22" s="7" t="s">
         <v>59</v>
       </c>
@@ -1790,7 +1879,9 @@
     </row>
     <row r="23" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-      <c r="C23" s="18"/>
+      <c r="C23" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D23" s="16" t="s">
         <v>174</v>
       </c>
@@ -1803,7 +1894,9 @@
       <c r="G23" s="13">
         <v>21</v>
       </c>
-      <c r="H23" s="13"/>
+      <c r="H23" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I23" s="7" t="s">
         <v>60</v>
       </c>
@@ -1826,7 +1919,9 @@
     </row>
     <row r="24" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
-      <c r="C24" s="18"/>
+      <c r="C24" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D24" s="16" t="s">
         <v>174</v>
       </c>
@@ -1839,7 +1934,9 @@
       <c r="G24" s="13">
         <v>22</v>
       </c>
-      <c r="H24" s="13"/>
+      <c r="H24" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I24" s="7" t="s">
         <v>61</v>
       </c>
@@ -1858,7 +1955,9 @@
     </row>
     <row r="25" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
-      <c r="C25" s="18"/>
+      <c r="C25" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D25" s="16" t="s">
         <v>174</v>
       </c>
@@ -1871,7 +1970,9 @@
       <c r="G25" s="13">
         <v>23</v>
       </c>
-      <c r="H25" s="13"/>
+      <c r="H25" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I25" s="7" t="s">
         <v>62</v>
       </c>
@@ -1896,7 +1997,9 @@
     </row>
     <row r="26" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
-      <c r="C26" s="18"/>
+      <c r="C26" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D26" s="16" t="s">
         <v>175</v>
       </c>
@@ -1909,7 +2012,9 @@
       <c r="G26" s="13">
         <v>24</v>
       </c>
-      <c r="H26" s="13"/>
+      <c r="H26" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I26" s="7" t="s">
         <v>63</v>
       </c>
@@ -1930,7 +2035,9 @@
     </row>
     <row r="27" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
-      <c r="C27" s="18"/>
+      <c r="C27" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="D27" s="16" t="s">
         <v>171</v>
       </c>
@@ -1943,7 +2050,9 @@
       <c r="G27" s="13">
         <v>25</v>
       </c>
-      <c r="H27" s="13"/>
+      <c r="H27" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I27" s="7" t="s">
         <v>64</v>
       </c>
@@ -1968,7 +2077,9 @@
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
-      <c r="C28" s="18"/>
+      <c r="C28" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D28" s="16" t="s">
         <v>174</v>
       </c>
@@ -1981,7 +2092,9 @@
       <c r="G28" s="13">
         <v>26</v>
       </c>
-      <c r="H28" s="13"/>
+      <c r="H28" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I28" s="8" t="s">
         <v>101</v>
       </c>
@@ -2002,7 +2115,9 @@
     </row>
     <row r="29" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
-      <c r="C29" s="18"/>
+      <c r="C29" s="18" t="s">
+        <v>181</v>
+      </c>
       <c r="D29" s="16" t="s">
         <v>175</v>
       </c>
@@ -2015,7 +2130,9 @@
       <c r="G29" s="13">
         <v>27</v>
       </c>
-      <c r="H29" s="13"/>
+      <c r="H29" s="13" t="s">
+        <v>174</v>
+      </c>
       <c r="I29" s="8" t="s">
         <v>103</v>
       </c>
@@ -2036,7 +2153,9 @@
     </row>
     <row r="30" spans="2:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
-      <c r="C30" s="18"/>
+      <c r="C30" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D30" s="16" t="s">
         <v>171</v>
       </c>
@@ -2049,7 +2168,9 @@
       <c r="G30" s="13">
         <v>28</v>
       </c>
-      <c r="H30" s="13"/>
+      <c r="H30" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I30" s="8" t="s">
         <v>106</v>
       </c>
@@ -2072,7 +2193,9 @@
     </row>
     <row r="31" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
-      <c r="C31" s="18"/>
+      <c r="C31" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D31" s="16" t="s">
         <v>171</v>
       </c>
@@ -2085,7 +2208,9 @@
       <c r="G31" s="13">
         <v>29</v>
       </c>
-      <c r="H31" s="13"/>
+      <c r="H31" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I31" s="8" t="s">
         <v>107</v>
       </c>
@@ -2106,14 +2231,18 @@
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
-      <c r="C32" s="18"/>
+      <c r="C32" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D32" s="16"/>
       <c r="E32" s="14"/>
       <c r="F32" s="12"/>
       <c r="G32" s="13">
         <v>30</v>
       </c>
-      <c r="H32" s="13"/>
+      <c r="H32" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I32" s="8" t="s">
         <v>108</v>
       </c>
@@ -2132,14 +2261,18 @@
     </row>
     <row r="33" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
-      <c r="C33" s="18"/>
+      <c r="C33" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D33" s="16"/>
       <c r="E33" s="14"/>
       <c r="F33" s="12"/>
       <c r="G33" s="13">
         <v>31</v>
       </c>
-      <c r="H33" s="13"/>
+      <c r="H33" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I33" s="8" t="s">
         <v>109</v>
       </c>
@@ -2160,7 +2293,9 @@
     </row>
     <row r="34" spans="2:15" ht="72" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
-      <c r="C34" s="18"/>
+      <c r="C34" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D34" s="16" t="s">
         <v>171</v>
       </c>
@@ -2173,7 +2308,9 @@
       <c r="G34" s="13">
         <v>32</v>
       </c>
-      <c r="H34" s="13"/>
+      <c r="H34" s="13" t="s">
+        <v>185</v>
+      </c>
       <c r="I34" s="8" t="s">
         <v>111</v>
       </c>
@@ -2196,14 +2333,18 @@
     </row>
     <row r="35" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
-      <c r="C35" s="18"/>
+      <c r="C35" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D35" s="16"/>
       <c r="E35" s="14"/>
       <c r="F35" s="12"/>
       <c r="G35" s="13">
         <v>33</v>
       </c>
-      <c r="H35" s="13"/>
+      <c r="H35" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I35" s="8" t="s">
         <v>142</v>
       </c>
@@ -2224,7 +2365,9 @@
     </row>
     <row r="36" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
-      <c r="C36" s="18"/>
+      <c r="C36" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D36" s="16" t="s">
         <v>171</v>
       </c>
@@ -2237,7 +2380,9 @@
       <c r="G36" s="13">
         <v>34</v>
       </c>
-      <c r="H36" s="13"/>
+      <c r="H36" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I36" s="8" t="s">
         <v>113</v>
       </c>
@@ -2262,7 +2407,9 @@
     </row>
     <row r="37" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
-      <c r="C37" s="18"/>
+      <c r="C37" s="18" t="s">
+        <v>182</v>
+      </c>
       <c r="D37" s="16" t="s">
         <v>173</v>
       </c>
@@ -2275,7 +2422,9 @@
       <c r="G37" s="13">
         <v>35</v>
       </c>
-      <c r="H37" s="13"/>
+      <c r="H37" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I37" s="8" t="s">
         <v>115</v>
       </c>
@@ -2298,7 +2447,9 @@
     </row>
     <row r="38" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
-      <c r="C38" s="18"/>
+      <c r="C38" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="D38" s="16" t="s">
         <v>171</v>
       </c>
@@ -2311,7 +2462,9 @@
       <c r="G38" s="13">
         <v>36</v>
       </c>
-      <c r="H38" s="13"/>
+      <c r="H38" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I38" s="8" t="s">
         <v>117</v>
       </c>
@@ -2332,7 +2485,9 @@
     </row>
     <row r="39" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
-      <c r="C39" s="18"/>
+      <c r="C39" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="D39" s="16" t="s">
         <v>171</v>
       </c>
@@ -2345,7 +2500,9 @@
       <c r="G39" s="13">
         <v>37</v>
       </c>
-      <c r="H39" s="13"/>
+      <c r="H39" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I39" s="8" t="s">
         <v>133</v>
       </c>
@@ -2366,14 +2523,18 @@
     </row>
     <row r="40" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
-      <c r="C40" s="18"/>
+      <c r="C40" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="D40" s="16"/>
       <c r="E40" s="14"/>
       <c r="F40" s="12"/>
       <c r="G40" s="13">
         <v>38</v>
       </c>
-      <c r="H40" s="13"/>
+      <c r="H40" s="13" t="s">
+        <v>184</v>
+      </c>
       <c r="I40" s="8" t="s">
         <v>134</v>
       </c>
@@ -2394,7 +2555,9 @@
     </row>
     <row r="41" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
-      <c r="C41" s="18"/>
+      <c r="C41" s="18" t="s">
+        <v>179</v>
+      </c>
       <c r="D41" s="16" t="s">
         <v>171</v>
       </c>
@@ -2407,7 +2570,9 @@
       <c r="G41" s="13">
         <v>39</v>
       </c>
-      <c r="H41" s="13"/>
+      <c r="H41" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I41" s="8" t="s">
         <v>137</v>
       </c>
@@ -2430,7 +2595,9 @@
     </row>
     <row r="42" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
-      <c r="C42" s="18"/>
+      <c r="C42" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="D42" s="16" t="s">
         <v>171</v>
       </c>
@@ -2443,7 +2610,9 @@
       <c r="G42" s="13">
         <v>40</v>
       </c>
-      <c r="H42" s="13"/>
+      <c r="H42" s="13" t="s">
+        <v>185</v>
+      </c>
       <c r="I42" s="8" t="s">
         <v>147</v>
       </c>
@@ -2464,7 +2633,9 @@
     </row>
     <row r="43" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
-      <c r="C43" s="18"/>
+      <c r="C43" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="D43" s="16" t="s">
         <v>171</v>
       </c>
@@ -2477,7 +2648,9 @@
       <c r="G43" s="13">
         <v>41</v>
       </c>
-      <c r="H43" s="13"/>
+      <c r="H43" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I43" s="8" t="s">
         <v>150</v>
       </c>
@@ -2498,7 +2671,9 @@
     </row>
     <row r="44" spans="2:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
-      <c r="C44" s="18"/>
+      <c r="C44" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="D44" s="16" t="s">
         <v>171</v>
       </c>
@@ -2511,7 +2686,9 @@
       <c r="G44" s="13">
         <v>42</v>
       </c>
-      <c r="H44" s="13"/>
+      <c r="H44" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I44" s="8" t="s">
         <v>153</v>
       </c>
@@ -2534,7 +2711,9 @@
     </row>
     <row r="45" spans="2:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
-      <c r="C45" s="18"/>
+      <c r="C45" s="18" t="s">
+        <v>180</v>
+      </c>
       <c r="D45" s="16" t="s">
         <v>171</v>
       </c>
@@ -2547,7 +2726,9 @@
       <c r="G45" s="13">
         <v>43</v>
       </c>
-      <c r="H45" s="13"/>
+      <c r="H45" s="13" t="s">
+        <v>183</v>
+      </c>
       <c r="I45" s="8" t="s">
         <v>157</v>
       </c>

</xml_diff>